<commit_message>
Update get code response and generate excel api
</commit_message>
<xml_diff>
--- a/media/excel/2020/TT1/Others.xlsx
+++ b/media/excel/2020/TT1/Others.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>SAP ID</t>
   </si>
@@ -43,10 +43,19 @@
     <t>Total</t>
   </si>
   <si>
+    <t>Evaluated</t>
+  </si>
+  <si>
     <t>001</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>002</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -423,14 +432,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="10" width="15" customWidth="1"/>
+    <col min="2" max="11" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -461,10 +470,13 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -493,10 +505,13 @@
       <c r="J2">
         <v>14</v>
       </c>
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -524,6 +539,9 @@
       </c>
       <c r="J3">
         <v>5</v>
+      </c>
+      <c r="K3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>